<commit_message>
added citation statistics snarfed from html pages
</commit_message>
<xml_diff>
--- a/beamline_publication_data.xlsx
+++ b/beamline_publication_data.xlsx
@@ -427,10 +427,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15.6" customWidth="1" min="4" max="4"/>
-    <col width="16.9" customWidth="1" min="5" max="5"/>
-    <col width="15.6" customWidth="1" min="6" max="6"/>
-    <col width="15.6" customWidth="1" min="7" max="7"/>
+    <col width="26" customWidth="1" min="3" max="3"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+    <col width="15.6" customWidth="1" min="5" max="5"/>
+    <col width="20.28" customWidth="1" min="6" max="6"/>
+    <col width="24.336" customWidth="1" min="7" max="7"/>
+    <col width="24.336" customWidth="1" min="8" max="8"/>
+    <col width="24.336" customWidth="1" min="9" max="9"/>
+    <col width="24.336" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -446,32 +450,44 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>program</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>total</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>high profile</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>years operating</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>% high profile</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>pubs per year</t>
         </is>
       </c>
-      <c r="H1" s="1" t="n"/>
-      <c r="I1" s="1" t="n"/>
-      <c r="J1" s="1" t="n"/>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>total citations</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>citations per paper</t>
+        </is>
+      </c>
       <c r="K1" s="1" t="n"/>
       <c r="L1" s="1" t="n"/>
       <c r="M1" s="1" t="n"/>
@@ -497,23 +513,31 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+          <t>Soft X-ray Scattering &amp; Spectroscopy</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>32</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2">
-        <f>D3/C3</f>
-        <v/>
+        <v>12</v>
+      </c>
+      <c r="F3" t="n">
+        <v>9</v>
       </c>
       <c r="G3" s="2">
-        <f>C3/E3</f>
+        <f>E3/D3</f>
+        <v/>
+      </c>
+      <c r="H3" s="2">
+        <f>D3/F3</f>
+        <v/>
+      </c>
+      <c r="I3" t="n">
+        <v>378</v>
+      </c>
+      <c r="J3" s="2">
+        <f>I3/D3</f>
         <v/>
       </c>
     </row>
@@ -530,23 +554,31 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>170</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
+          <t>Imaging</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>194</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2">
-        <f>D4/C4</f>
-        <v/>
+        <v>51</v>
+      </c>
+      <c r="F4" t="n">
+        <v>13</v>
       </c>
       <c r="G4" s="2">
-        <f>C4/E4</f>
+        <f>E4/D4</f>
+        <v/>
+      </c>
+      <c r="H4" s="2">
+        <f>D4/F4</f>
+        <v/>
+      </c>
+      <c r="I4" t="n">
+        <v>3675</v>
+      </c>
+      <c r="J4" s="2">
+        <f>I4/D4</f>
         <v/>
       </c>
     </row>
@@ -563,23 +595,31 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>78</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
+          <t>Imaging</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>99</v>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F5" s="2">
-        <f>D5/C5</f>
-        <v/>
+        <v>24</v>
+      </c>
+      <c r="F5" t="n">
+        <v>7</v>
       </c>
       <c r="G5" s="2">
-        <f>C5/E5</f>
+        <f>E5/D5</f>
+        <v/>
+      </c>
+      <c r="H5" s="2">
+        <f>D5/F5</f>
+        <v/>
+      </c>
+      <c r="I5" t="n">
+        <v>895</v>
+      </c>
+      <c r="J5" s="2">
+        <f>I5/D5</f>
         <v/>
       </c>
     </row>
@@ -596,23 +636,31 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+          <t>Complex Scattering</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>38</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
-      </c>
-      <c r="F6" s="2">
-        <f>D6/C6</f>
-        <v/>
+        <v>11</v>
+      </c>
+      <c r="F6" t="n">
+        <v>6</v>
       </c>
       <c r="G6" s="2">
-        <f>C6/E6</f>
+        <f>E6/D6</f>
+        <v/>
+      </c>
+      <c r="H6" s="2">
+        <f>D6/F6</f>
+        <v/>
+      </c>
+      <c r="I6" t="n">
+        <v>415</v>
+      </c>
+      <c r="J6" s="2">
+        <f>I6/D6</f>
         <v/>
       </c>
     </row>
@@ -629,23 +677,31 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>89</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>29</t>
-        </is>
+          <t>Imaging</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>99</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2">
-        <f>D7/C7</f>
-        <v/>
+        <v>28</v>
+      </c>
+      <c r="F7" t="n">
+        <v>11</v>
       </c>
       <c r="G7" s="2">
-        <f>C7/E7</f>
+        <f>E7/D7</f>
+        <v/>
+      </c>
+      <c r="H7" s="2">
+        <f>D7/F7</f>
+        <v/>
+      </c>
+      <c r="I7" t="n">
+        <v>2262</v>
+      </c>
+      <c r="J7" s="2">
+        <f>I7/D7</f>
         <v/>
       </c>
     </row>
@@ -662,23 +718,31 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>122</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
+          <t>Hard X-ray Scattering &amp; Spectroscopy</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>145</v>
       </c>
       <c r="E8" t="n">
-        <v>6</v>
-      </c>
-      <c r="F8" s="2">
-        <f>D8/C8</f>
-        <v/>
+        <v>47</v>
+      </c>
+      <c r="F8" t="n">
+        <v>7</v>
       </c>
       <c r="G8" s="2">
-        <f>C8/E8</f>
+        <f>E8/D8</f>
+        <v/>
+      </c>
+      <c r="H8" s="2">
+        <f>D8/F8</f>
+        <v/>
+      </c>
+      <c r="I8" t="n">
+        <v>2019</v>
+      </c>
+      <c r="J8" s="2">
+        <f>I8/D8</f>
         <v/>
       </c>
     </row>
@@ -695,23 +759,31 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>341</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>239</t>
-        </is>
+          <t>Hard X-ray Scattering &amp; Spectroscopy</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>445</v>
       </c>
       <c r="E9" t="n">
-        <v>6</v>
-      </c>
-      <c r="F9" s="2">
-        <f>D9/C9</f>
-        <v/>
+        <v>310</v>
+      </c>
+      <c r="F9" t="n">
+        <v>7</v>
       </c>
       <c r="G9" s="2">
-        <f>C9/E9</f>
+        <f>E9/D9</f>
+        <v/>
+      </c>
+      <c r="H9" s="2">
+        <f>D9/F9</f>
+        <v/>
+      </c>
+      <c r="I9" t="n">
+        <v>14526</v>
+      </c>
+      <c r="J9" s="2">
+        <f>I9/D9</f>
         <v/>
       </c>
     </row>
@@ -728,23 +800,31 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>46</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+          <t>Soft X-ray Scattering &amp; Spectroscopy</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>52</v>
       </c>
       <c r="E10" t="n">
-        <v>6</v>
-      </c>
-      <c r="F10" s="2">
-        <f>D10/C10</f>
-        <v/>
+        <v>28</v>
+      </c>
+      <c r="F10" t="n">
+        <v>7</v>
       </c>
       <c r="G10" s="2">
-        <f>C10/E10</f>
+        <f>E10/D10</f>
+        <v/>
+      </c>
+      <c r="H10" s="2">
+        <f>D10/F10</f>
+        <v/>
+      </c>
+      <c r="I10" t="n">
+        <v>1904</v>
+      </c>
+      <c r="J10" s="2">
+        <f>I10/D10</f>
         <v/>
       </c>
     </row>
@@ -761,23 +841,31 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>32</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+          <t>Soft X-ray Scattering &amp; Spectroscopy</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>39</v>
       </c>
       <c r="E11" t="n">
-        <v>5</v>
-      </c>
-      <c r="F11" s="2">
-        <f>D11/C11</f>
-        <v/>
+        <v>18</v>
+      </c>
+      <c r="F11" t="n">
+        <v>6</v>
       </c>
       <c r="G11" s="2">
-        <f>C11/E11</f>
+        <f>E11/D11</f>
+        <v/>
+      </c>
+      <c r="H11" s="2">
+        <f>D11/F11</f>
+        <v/>
+      </c>
+      <c r="I11" t="n">
+        <v>344</v>
+      </c>
+      <c r="J11" s="2">
+        <f>I11/D11</f>
         <v/>
       </c>
     </row>
@@ -794,23 +882,31 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>81</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>33</t>
-        </is>
+          <t>Imaging</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>106</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
-      </c>
-      <c r="F12" s="2">
-        <f>D12/C12</f>
-        <v/>
+        <v>39</v>
+      </c>
+      <c r="F12" t="n">
+        <v>9</v>
       </c>
       <c r="G12" s="2">
-        <f>C12/E12</f>
+        <f>E12/D12</f>
+        <v/>
+      </c>
+      <c r="H12" s="2">
+        <f>D12/F12</f>
+        <v/>
+      </c>
+      <c r="I12" t="n">
+        <v>1768</v>
+      </c>
+      <c r="J12" s="2">
+        <f>I12/D12</f>
         <v/>
       </c>
     </row>
@@ -827,23 +923,31 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>233</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>133</t>
-        </is>
+          <t>Hard X-ray Scattering &amp; Spectroscopy</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>270</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
-      </c>
-      <c r="F13" s="2">
-        <f>D13/C13</f>
-        <v/>
+        <v>148</v>
+      </c>
+      <c r="F13" t="n">
+        <v>9</v>
       </c>
       <c r="G13" s="2">
-        <f>C13/E13</f>
+        <f>E13/D13</f>
+        <v/>
+      </c>
+      <c r="H13" s="2">
+        <f>D13/F13</f>
+        <v/>
+      </c>
+      <c r="I13" t="n">
+        <v>13805</v>
+      </c>
+      <c r="J13" s="2">
+        <f>I13/D13</f>
         <v/>
       </c>
     </row>
@@ -860,23 +964,31 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>34</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+          <t>Complex Scattering</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>36</v>
       </c>
       <c r="E14" t="n">
-        <v>14</v>
-      </c>
-      <c r="F14" s="2">
-        <f>D14/C14</f>
-        <v/>
+        <v>6</v>
+      </c>
+      <c r="F14" t="n">
+        <v>15</v>
       </c>
       <c r="G14" s="2">
-        <f>C14/E14</f>
+        <f>E14/D14</f>
+        <v/>
+      </c>
+      <c r="H14" s="2">
+        <f>D14/F14</f>
+        <v/>
+      </c>
+      <c r="I14" t="n">
+        <v>173</v>
+      </c>
+      <c r="J14" s="2">
+        <f>I14/D14</f>
         <v/>
       </c>
     </row>
@@ -893,23 +1005,31 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>402</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>186</t>
-        </is>
+          <t>Complex Scattering</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>463</v>
       </c>
       <c r="E15" t="n">
-        <v>7</v>
-      </c>
-      <c r="F15" s="2">
-        <f>D15/C15</f>
-        <v/>
+        <v>224</v>
+      </c>
+      <c r="F15" t="n">
+        <v>8</v>
       </c>
       <c r="G15" s="2">
-        <f>C15/E15</f>
+        <f>E15/D15</f>
+        <v/>
+      </c>
+      <c r="H15" s="2">
+        <f>D15/F15</f>
+        <v/>
+      </c>
+      <c r="I15" t="n">
+        <v>10663</v>
+      </c>
+      <c r="J15" s="2">
+        <f>I15/D15</f>
         <v/>
       </c>
     </row>
@@ -926,23 +1046,31 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>66</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+          <t>Complex Scattering</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>76</v>
       </c>
       <c r="E16" t="n">
-        <v>9</v>
-      </c>
-      <c r="F16" s="2">
-        <f>D16/C16</f>
-        <v/>
+        <v>14</v>
+      </c>
+      <c r="F16" t="n">
+        <v>10</v>
       </c>
       <c r="G16" s="2">
-        <f>C16/E16</f>
+        <f>E16/D16</f>
+        <v/>
+      </c>
+      <c r="H16" s="2">
+        <f>D16/F16</f>
+        <v/>
+      </c>
+      <c r="I16" t="n">
+        <v>671</v>
+      </c>
+      <c r="J16" s="2">
+        <f>I16/D16</f>
         <v/>
       </c>
     </row>
@@ -959,23 +1087,31 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>140</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+          <t>Complex Scattering</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>171</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
-      </c>
-      <c r="F17" s="2">
-        <f>D17/C17</f>
-        <v/>
+        <v>60</v>
+      </c>
+      <c r="F17" t="n">
+        <v>9</v>
       </c>
       <c r="G17" s="2">
-        <f>C17/E17</f>
+        <f>E17/D17</f>
+        <v/>
+      </c>
+      <c r="H17" s="2">
+        <f>D17/F17</f>
+        <v/>
+      </c>
+      <c r="I17" t="n">
+        <v>1618</v>
+      </c>
+      <c r="J17" s="2">
+        <f>I17/D17</f>
         <v/>
       </c>
     </row>
@@ -992,23 +1128,31 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>124</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
+          <t>Structural Biology</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>166</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
-      </c>
-      <c r="F18" s="2">
-        <f>D18/C18</f>
-        <v/>
+        <v>40</v>
+      </c>
+      <c r="F18" t="n">
+        <v>11</v>
       </c>
       <c r="G18" s="2">
-        <f>C18/E18</f>
+        <f>E18/D18</f>
+        <v/>
+      </c>
+      <c r="H18" s="2">
+        <f>D18/F18</f>
+        <v/>
+      </c>
+      <c r="I18" t="n">
+        <v>1953</v>
+      </c>
+      <c r="J18" s="2">
+        <f>I18/D18</f>
         <v/>
       </c>
     </row>
@@ -1025,23 +1169,31 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>29</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+          <t>Structural Biology</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>32</v>
       </c>
       <c r="E19" t="n">
-        <v>7</v>
-      </c>
-      <c r="F19" s="2">
-        <f>D19/C19</f>
-        <v/>
+        <v>3</v>
+      </c>
+      <c r="F19" t="n">
+        <v>8</v>
       </c>
       <c r="G19" s="2">
-        <f>C19/E19</f>
+        <f>E19/D19</f>
+        <v/>
+      </c>
+      <c r="H19" s="2">
+        <f>D19/F19</f>
+        <v/>
+      </c>
+      <c r="I19" t="n">
+        <v>315</v>
+      </c>
+      <c r="J19" s="2">
+        <f>I19/D19</f>
         <v/>
       </c>
     </row>
@@ -1058,23 +1210,31 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>227</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>102</t>
-        </is>
+          <t>Structural Biology</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>282</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
-      </c>
-      <c r="F20" s="2">
-        <f>D20/C20</f>
-        <v/>
+        <v>109</v>
+      </c>
+      <c r="F20" t="n">
+        <v>11</v>
       </c>
       <c r="G20" s="2">
-        <f>C20/E20</f>
+        <f>E20/D20</f>
+        <v/>
+      </c>
+      <c r="H20" s="2">
+        <f>D20/F20</f>
+        <v/>
+      </c>
+      <c r="I20" t="n">
+        <v>4433</v>
+      </c>
+      <c r="J20" s="2">
+        <f>I20/D20</f>
         <v/>
       </c>
     </row>
@@ -1091,23 +1251,31 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>169</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>77</t>
-        </is>
+          <t>Structural Biology</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>203</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
-      </c>
-      <c r="F21" s="2">
-        <f>D21/C21</f>
-        <v/>
+        <v>82</v>
+      </c>
+      <c r="F21" t="n">
+        <v>11</v>
       </c>
       <c r="G21" s="2">
-        <f>C21/E21</f>
+        <f>E21/D21</f>
+        <v/>
+      </c>
+      <c r="H21" s="2">
+        <f>D21/F21</f>
+        <v/>
+      </c>
+      <c r="I21" t="n">
+        <v>3257</v>
+      </c>
+      <c r="J21" s="2">
+        <f>I21/D21</f>
         <v/>
       </c>
     </row>
@@ -1124,23 +1292,31 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>93</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>59</t>
-        </is>
+          <t>Imaging</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>104</v>
       </c>
       <c r="E22" t="n">
-        <v>7</v>
-      </c>
-      <c r="F22" s="2">
-        <f>D22/C22</f>
-        <v/>
+        <v>68</v>
+      </c>
+      <c r="F22" t="n">
+        <v>8</v>
       </c>
       <c r="G22" s="2">
-        <f>C22/E22</f>
+        <f>E22/D22</f>
+        <v/>
+      </c>
+      <c r="H22" s="2">
+        <f>D22/F22</f>
+        <v/>
+      </c>
+      <c r="I22" t="n">
+        <v>3764</v>
+      </c>
+      <c r="J22" s="2">
+        <f>I22/D22</f>
         <v/>
       </c>
     </row>
@@ -1157,23 +1333,31 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+          <t>Structural Biology</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>21</v>
       </c>
       <c r="E23" t="n">
-        <v>6</v>
-      </c>
-      <c r="F23" s="2">
-        <f>D23/C23</f>
-        <v/>
+        <v>4</v>
+      </c>
+      <c r="F23" t="n">
+        <v>7</v>
       </c>
       <c r="G23" s="2">
-        <f>C23/E23</f>
+        <f>E23/D23</f>
+        <v/>
+      </c>
+      <c r="H23" s="2">
+        <f>D23/F23</f>
+        <v/>
+      </c>
+      <c r="I23" t="n">
+        <v>190</v>
+      </c>
+      <c r="J23" s="2">
+        <f>I23/D23</f>
         <v/>
       </c>
     </row>
@@ -1190,23 +1374,31 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>54</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+          <t>Soft X-ray Scattering &amp; Spectroscopy</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>68</v>
       </c>
       <c r="E24" t="n">
-        <v>6</v>
-      </c>
-      <c r="F24" s="2">
-        <f>D24/C24</f>
-        <v/>
+        <v>32</v>
+      </c>
+      <c r="F24" t="n">
+        <v>7</v>
       </c>
       <c r="G24" s="2">
-        <f>C24/E24</f>
+        <f>E24/D24</f>
+        <v/>
+      </c>
+      <c r="H24" s="2">
+        <f>D24/F24</f>
+        <v/>
+      </c>
+      <c r="I24" t="n">
+        <v>1242</v>
+      </c>
+      <c r="J24" s="2">
+        <f>I24/D24</f>
         <v/>
       </c>
     </row>
@@ -1223,23 +1415,31 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>47</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+          <t>Soft X-ray Scattering &amp; Spectroscopy</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>51</v>
       </c>
       <c r="E25" t="n">
-        <v>7</v>
-      </c>
-      <c r="F25" s="2">
-        <f>D25/C25</f>
-        <v/>
+        <v>21</v>
+      </c>
+      <c r="F25" t="n">
+        <v>8</v>
       </c>
       <c r="G25" s="2">
-        <f>C25/E25</f>
+        <f>E25/D25</f>
+        <v/>
+      </c>
+      <c r="H25" s="2">
+        <f>D25/F25</f>
+        <v/>
+      </c>
+      <c r="I25" t="n">
+        <v>1153</v>
+      </c>
+      <c r="J25" s="2">
+        <f>I25/D25</f>
         <v/>
       </c>
     </row>
@@ -1256,23 +1456,31 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>Soft X-ray Scattering &amp; Spectroscopy</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>7</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2">
-        <f>D26/C26</f>
-        <v/>
+        <v>2</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2</v>
       </c>
       <c r="G26" s="2">
-        <f>C26/E26</f>
+        <f>E26/D26</f>
+        <v/>
+      </c>
+      <c r="H26" s="2">
+        <f>D26/F26</f>
+        <v/>
+      </c>
+      <c r="I26" t="n">
+        <v>32</v>
+      </c>
+      <c r="J26" s="2">
+        <f>I26/D26</f>
         <v/>
       </c>
     </row>
@@ -1289,23 +1497,31 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>37</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+          <t>Soft X-ray Scattering &amp; Spectroscopy</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>41</v>
       </c>
       <c r="E27" t="n">
-        <v>9</v>
-      </c>
-      <c r="F27" s="2">
-        <f>D27/C27</f>
-        <v/>
+        <v>18</v>
+      </c>
+      <c r="F27" t="n">
+        <v>10</v>
       </c>
       <c r="G27" s="2">
-        <f>C27/E27</f>
+        <f>E27/D27</f>
+        <v/>
+      </c>
+      <c r="H27" s="2">
+        <f>D27/F27</f>
+        <v/>
+      </c>
+      <c r="I27" t="n">
+        <v>611</v>
+      </c>
+      <c r="J27" s="2">
+        <f>I27/D27</f>
         <v/>
       </c>
     </row>
@@ -1322,23 +1538,31 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>136</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>70</t>
-        </is>
+          <t>Soft X-ray Scattering &amp; Spectroscopy</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>160</v>
       </c>
       <c r="E28" t="n">
-        <v>9</v>
-      </c>
-      <c r="F28" s="2">
-        <f>D28/C28</f>
-        <v/>
+        <v>87</v>
+      </c>
+      <c r="F28" t="n">
+        <v>10</v>
       </c>
       <c r="G28" s="2">
-        <f>C28/E28</f>
+        <f>E28/D28</f>
+        <v/>
+      </c>
+      <c r="H28" s="2">
+        <f>D28/F28</f>
+        <v/>
+      </c>
+      <c r="I28" t="n">
+        <v>4577</v>
+      </c>
+      <c r="J28" s="2">
+        <f>I28/D28</f>
         <v/>
       </c>
     </row>
@@ -1355,23 +1579,31 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>Hard X-ray Scattering &amp; Spectroscopy</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>4</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
-      </c>
-      <c r="F29" s="2">
-        <f>D29/C29</f>
-        <v/>
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>3</v>
       </c>
       <c r="G29" s="2">
-        <f>C29/E29</f>
+        <f>E29/D29</f>
+        <v/>
+      </c>
+      <c r="H29" s="2">
+        <f>D29/F29</f>
+        <v/>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2">
+        <f>I29/D29</f>
         <v/>
       </c>
     </row>
@@ -1388,23 +1620,31 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>139</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>57</t>
-        </is>
+          <t>Hard X-ray Scattering &amp; Spectroscopy</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>166</v>
       </c>
       <c r="E30" t="n">
-        <v>7</v>
-      </c>
-      <c r="F30" s="2">
-        <f>D30/C30</f>
-        <v/>
+        <v>73</v>
+      </c>
+      <c r="F30" t="n">
+        <v>9</v>
       </c>
       <c r="G30" s="2">
-        <f>C30/E30</f>
+        <f>E30/D30</f>
+        <v/>
+      </c>
+      <c r="H30" s="2">
+        <f>D30/F30</f>
+        <v/>
+      </c>
+      <c r="I30" t="n">
+        <v>2950</v>
+      </c>
+      <c r="J30" s="2">
+        <f>I30/D30</f>
         <v/>
       </c>
     </row>
@@ -1421,23 +1661,31 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>323</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>144</t>
-        </is>
+          <t>Hard X-ray Scattering &amp; Spectroscopy</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>356</v>
       </c>
       <c r="E31" t="n">
-        <v>10</v>
-      </c>
-      <c r="F31" s="2">
-        <f>D31/C31</f>
-        <v/>
+        <v>159</v>
+      </c>
+      <c r="F31" t="n">
+        <v>12</v>
       </c>
       <c r="G31" s="2">
-        <f>C31/E31</f>
+        <f>E31/D31</f>
+        <v/>
+      </c>
+      <c r="H31" s="2">
+        <f>D31/F31</f>
+        <v/>
+      </c>
+      <c r="I31" t="n">
+        <v>11743</v>
+      </c>
+      <c r="J31" s="2">
+        <f>I31/D31</f>
         <v/>
       </c>
     </row>

</xml_diff>